<commit_message>
changes made in local recent revised
</commit_message>
<xml_diff>
--- a/data/TC01_Signin.xlsx
+++ b/data/TC01_Signin.xlsx
@@ -23,10 +23,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>udhayasundar</t>
+    <t>TestEsri</t>
   </si>
   <si>
-    <t>udy$12345</t>
+    <t>Test@12345</t>
   </si>
 </sst>
 </file>
@@ -36,11 +36,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -56,6 +57,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,8 +108,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -120,18 +132,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -142,15 +156,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="Test@12345"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>